<commit_message>
ya el valor de uk esta
</commit_message>
<xml_diff>
--- a/matriz_puntos.xlsx
+++ b/matriz_puntos.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:ER5"/>
+  <dimension ref="A1:ER7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1766,898 +1766,1496 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>hk</t>
-        </is>
-      </c>
-      <c r="B4" t="n">
-        <v>1</v>
-      </c>
-      <c r="C4" t="n">
-        <v>1</v>
-      </c>
-      <c r="D4" t="n">
-        <v>1</v>
-      </c>
-      <c r="E4" t="n">
-        <v>1</v>
-      </c>
-      <c r="F4" t="n">
-        <v>1</v>
-      </c>
-      <c r="G4" t="n">
-        <v>5</v>
-      </c>
-      <c r="H4" t="n">
-        <v>1</v>
-      </c>
-      <c r="I4" t="n">
-        <v>1</v>
-      </c>
-      <c r="J4" t="n">
-        <v>1</v>
-      </c>
-      <c r="K4" t="n">
-        <v>1</v>
-      </c>
-      <c r="L4" t="n">
-        <v>1</v>
-      </c>
-      <c r="M4" t="n">
-        <v>1</v>
-      </c>
-      <c r="N4" t="n">
-        <v>1</v>
-      </c>
-      <c r="O4" t="n">
-        <v>10</v>
-      </c>
-      <c r="P4" t="n">
-        <v>1</v>
-      </c>
-      <c r="Q4" t="n">
-        <v>1</v>
-      </c>
-      <c r="R4" t="n">
-        <v>1</v>
-      </c>
-      <c r="S4" t="n">
-        <v>1</v>
-      </c>
-      <c r="T4" t="n">
-        <v>1</v>
-      </c>
-      <c r="U4" t="n">
-        <v>1</v>
-      </c>
-      <c r="V4" t="n">
-        <v>2</v>
-      </c>
-      <c r="W4" t="n">
-        <v>1</v>
-      </c>
-      <c r="X4" t="n">
-        <v>16</v>
-      </c>
-      <c r="Y4" t="n">
-        <v>1</v>
-      </c>
-      <c r="Z4" t="n">
-        <v>1</v>
-      </c>
-      <c r="AA4" t="n">
-        <v>1</v>
-      </c>
-      <c r="AB4" t="n">
-        <v>2</v>
-      </c>
-      <c r="AC4" t="n">
-        <v>1</v>
-      </c>
-      <c r="AD4" t="n">
-        <v>1</v>
-      </c>
-      <c r="AE4" t="n">
-        <v>1</v>
-      </c>
-      <c r="AF4" t="n">
-        <v>1</v>
-      </c>
-      <c r="AG4" t="n">
-        <v>1</v>
-      </c>
-      <c r="AH4" t="n">
-        <v>1</v>
-      </c>
-      <c r="AI4" t="n">
-        <v>1</v>
-      </c>
-      <c r="AJ4" t="n">
-        <v>1</v>
-      </c>
-      <c r="AK4" t="n">
-        <v>1</v>
-      </c>
-      <c r="AL4" t="n">
-        <v>1</v>
-      </c>
-      <c r="AM4" t="n">
-        <v>1</v>
-      </c>
-      <c r="AN4" t="n">
-        <v>1</v>
-      </c>
-      <c r="AO4" t="n">
-        <v>1</v>
-      </c>
-      <c r="AP4" t="n">
-        <v>1</v>
-      </c>
-      <c r="AQ4" t="n">
-        <v>1</v>
-      </c>
-      <c r="AR4" t="n">
-        <v>1</v>
-      </c>
-      <c r="AS4" t="n">
-        <v>1</v>
-      </c>
-      <c r="AT4" t="n">
-        <v>2</v>
-      </c>
-      <c r="AU4" t="n">
-        <v>1</v>
-      </c>
-      <c r="AV4" t="n">
-        <v>3</v>
-      </c>
-      <c r="AW4" t="n">
-        <v>1</v>
-      </c>
-      <c r="AX4" t="n">
-        <v>3</v>
-      </c>
-      <c r="AY4" t="n">
-        <v>1</v>
-      </c>
-      <c r="AZ4" t="n">
-        <v>1</v>
-      </c>
-      <c r="BA4" t="n">
-        <v>1</v>
-      </c>
-      <c r="BB4" t="n">
-        <v>1</v>
-      </c>
-      <c r="BC4" t="n">
-        <v>1</v>
-      </c>
-      <c r="BD4" t="n">
-        <v>1</v>
-      </c>
-      <c r="BE4" t="n">
-        <v>1</v>
-      </c>
-      <c r="BF4" t="n">
-        <v>1</v>
-      </c>
-      <c r="BG4" t="n">
-        <v>1</v>
-      </c>
-      <c r="BH4" t="n">
-        <v>1</v>
-      </c>
-      <c r="BI4" t="n">
-        <v>2</v>
-      </c>
-      <c r="BJ4" t="n">
-        <v>1</v>
-      </c>
-      <c r="BK4" t="n">
-        <v>1</v>
-      </c>
-      <c r="BL4" t="n">
-        <v>1</v>
-      </c>
-      <c r="BM4" t="n">
-        <v>2</v>
-      </c>
-      <c r="BN4" t="n">
-        <v>1</v>
-      </c>
-      <c r="BO4" t="n">
-        <v>1</v>
-      </c>
-      <c r="BP4" t="n">
-        <v>5</v>
-      </c>
-      <c r="BQ4" t="n">
-        <v>1</v>
-      </c>
-      <c r="BR4" t="n">
-        <v>5</v>
-      </c>
-      <c r="BS4" t="n">
-        <v>1</v>
-      </c>
-      <c r="BT4" t="n">
-        <v>1</v>
-      </c>
-      <c r="BU4" t="n">
-        <v>1</v>
-      </c>
-      <c r="BV4" t="n">
-        <v>1</v>
-      </c>
-      <c r="BW4" t="n">
-        <v>1</v>
-      </c>
-      <c r="BX4" t="n">
-        <v>1</v>
-      </c>
-      <c r="BY4" t="n">
-        <v>1</v>
-      </c>
-      <c r="BZ4" t="n">
-        <v>1</v>
-      </c>
-      <c r="CA4" t="n">
-        <v>1</v>
-      </c>
-      <c r="CB4" t="n">
-        <v>1</v>
-      </c>
-      <c r="CC4" t="n">
-        <v>1</v>
-      </c>
-      <c r="CD4" t="n">
-        <v>1</v>
-      </c>
-      <c r="CE4" t="n">
-        <v>1</v>
-      </c>
-      <c r="CF4" t="n">
-        <v>1</v>
-      </c>
-      <c r="CG4" t="n">
-        <v>1</v>
-      </c>
-      <c r="CH4" t="n">
-        <v>1</v>
-      </c>
-      <c r="CI4" t="n">
-        <v>1</v>
-      </c>
-      <c r="CJ4" t="n">
-        <v>1</v>
-      </c>
-      <c r="CK4" t="n">
-        <v>1</v>
-      </c>
-      <c r="CL4" t="n">
-        <v>1</v>
-      </c>
-      <c r="CM4" t="n">
-        <v>1</v>
-      </c>
-      <c r="CN4" t="n">
-        <v>1</v>
-      </c>
-      <c r="CO4" t="n">
-        <v>1</v>
-      </c>
-      <c r="CP4" t="n">
-        <v>1</v>
-      </c>
-      <c r="CQ4" t="n">
-        <v>1</v>
-      </c>
-      <c r="CR4" t="n">
-        <v>1</v>
-      </c>
-      <c r="CS4" t="n">
-        <v>1</v>
-      </c>
-      <c r="CT4" t="n">
-        <v>1</v>
-      </c>
-      <c r="CU4" t="n">
-        <v>1</v>
-      </c>
-      <c r="CV4" t="n">
-        <v>1</v>
-      </c>
-      <c r="CW4" t="n">
-        <v>1</v>
-      </c>
-      <c r="CX4" t="n">
-        <v>1</v>
-      </c>
-      <c r="CY4" t="n">
-        <v>2</v>
-      </c>
-      <c r="CZ4" t="n">
-        <v>2</v>
-      </c>
-      <c r="DA4" t="n">
-        <v>2</v>
-      </c>
-      <c r="DB4" t="n">
-        <v>1</v>
-      </c>
-      <c r="DC4" t="n">
-        <v>1</v>
-      </c>
-      <c r="DD4" t="n">
-        <v>1</v>
-      </c>
-      <c r="DE4" t="n">
-        <v>1</v>
-      </c>
-      <c r="DF4" t="n">
-        <v>1</v>
-      </c>
-      <c r="DG4" t="n">
-        <v>1</v>
-      </c>
-      <c r="DH4" t="n">
-        <v>1</v>
-      </c>
-      <c r="DI4" t="n">
-        <v>4</v>
-      </c>
-      <c r="DJ4" t="n">
-        <v>1</v>
-      </c>
-      <c r="DK4" t="n">
-        <v>1</v>
-      </c>
-      <c r="DL4" t="n">
-        <v>6</v>
-      </c>
-      <c r="DM4" t="n">
-        <v>1</v>
-      </c>
-      <c r="DN4" t="n">
-        <v>3</v>
-      </c>
-      <c r="DO4" t="n">
-        <v>1</v>
-      </c>
-      <c r="DP4" t="n">
-        <v>1</v>
-      </c>
-      <c r="DQ4" t="n">
-        <v>1</v>
-      </c>
-      <c r="DR4" t="n">
-        <v>2</v>
-      </c>
-      <c r="DS4" t="n">
-        <v>1</v>
-      </c>
-      <c r="DT4" t="n">
-        <v>1</v>
-      </c>
-      <c r="DU4" t="n">
-        <v>1</v>
-      </c>
-      <c r="DV4" t="n">
-        <v>1</v>
-      </c>
-      <c r="DW4" t="n">
-        <v>4</v>
-      </c>
-      <c r="DX4" t="n">
-        <v>1</v>
-      </c>
-      <c r="DY4" t="n">
-        <v>1</v>
-      </c>
-      <c r="DZ4" t="n">
-        <v>1</v>
-      </c>
-      <c r="EA4" t="n">
-        <v>1</v>
-      </c>
-      <c r="EB4" t="n">
-        <v>1</v>
-      </c>
-      <c r="EC4" t="n">
-        <v>1</v>
-      </c>
-      <c r="ED4" t="n">
-        <v>1</v>
-      </c>
-      <c r="EE4" t="n">
-        <v>1</v>
-      </c>
-      <c r="EF4" t="n">
-        <v>1</v>
-      </c>
-      <c r="EG4" t="n">
-        <v>1</v>
-      </c>
-      <c r="EH4" t="n">
-        <v>1</v>
-      </c>
-      <c r="EI4" t="n">
-        <v>1</v>
-      </c>
-      <c r="EJ4" t="n">
-        <v>2</v>
-      </c>
-      <c r="EK4" t="n">
-        <v>1</v>
-      </c>
-      <c r="EL4" t="n">
-        <v>1</v>
-      </c>
-      <c r="EM4" t="n">
-        <v>1</v>
-      </c>
-      <c r="EN4" t="n">
-        <v>6</v>
-      </c>
-      <c r="EO4" t="n">
-        <v>2</v>
-      </c>
-      <c r="EP4" t="n">
-        <v>1</v>
-      </c>
-      <c r="EQ4" t="n">
-        <v>1</v>
-      </c>
-      <c r="ER4" t="n">
-        <v>0</v>
-      </c>
+      <c r="A4" t="inlineStr"/>
+      <c r="B4" t="inlineStr"/>
+      <c r="C4" t="inlineStr"/>
+      <c r="D4" t="inlineStr"/>
+      <c r="E4" t="inlineStr"/>
+      <c r="F4" t="inlineStr"/>
+      <c r="G4" t="inlineStr"/>
+      <c r="H4" t="inlineStr"/>
+      <c r="I4" t="inlineStr"/>
+      <c r="J4" t="inlineStr"/>
+      <c r="K4" t="inlineStr"/>
+      <c r="L4" t="inlineStr"/>
+      <c r="M4" t="inlineStr"/>
+      <c r="N4" t="inlineStr"/>
+      <c r="O4" t="inlineStr"/>
+      <c r="P4" t="inlineStr"/>
+      <c r="Q4" t="inlineStr"/>
+      <c r="R4" t="inlineStr"/>
+      <c r="S4" t="inlineStr"/>
+      <c r="T4" t="inlineStr"/>
+      <c r="U4" t="inlineStr"/>
+      <c r="V4" t="inlineStr"/>
+      <c r="W4" t="inlineStr"/>
+      <c r="X4" t="inlineStr"/>
+      <c r="Y4" t="inlineStr"/>
+      <c r="Z4" t="inlineStr"/>
+      <c r="AA4" t="inlineStr"/>
+      <c r="AB4" t="inlineStr"/>
+      <c r="AC4" t="inlineStr"/>
+      <c r="AD4" t="inlineStr"/>
+      <c r="AE4" t="inlineStr"/>
+      <c r="AF4" t="inlineStr"/>
+      <c r="AG4" t="inlineStr"/>
+      <c r="AH4" t="inlineStr"/>
+      <c r="AI4" t="inlineStr"/>
+      <c r="AJ4" t="inlineStr"/>
+      <c r="AK4" t="inlineStr"/>
+      <c r="AL4" t="inlineStr"/>
+      <c r="AM4" t="inlineStr"/>
+      <c r="AN4" t="inlineStr"/>
+      <c r="AO4" t="inlineStr"/>
+      <c r="AP4" t="inlineStr"/>
+      <c r="AQ4" t="inlineStr"/>
+      <c r="AR4" t="inlineStr"/>
+      <c r="AS4" t="inlineStr"/>
+      <c r="AT4" t="inlineStr"/>
+      <c r="AU4" t="inlineStr"/>
+      <c r="AV4" t="inlineStr"/>
+      <c r="AW4" t="inlineStr"/>
+      <c r="AX4" t="inlineStr"/>
+      <c r="AY4" t="inlineStr"/>
+      <c r="AZ4" t="inlineStr"/>
+      <c r="BA4" t="inlineStr"/>
+      <c r="BB4" t="inlineStr"/>
+      <c r="BC4" t="inlineStr"/>
+      <c r="BD4" t="inlineStr"/>
+      <c r="BE4" t="inlineStr"/>
+      <c r="BF4" t="inlineStr"/>
+      <c r="BG4" t="inlineStr"/>
+      <c r="BH4" t="inlineStr"/>
+      <c r="BI4" t="inlineStr"/>
+      <c r="BJ4" t="inlineStr"/>
+      <c r="BK4" t="inlineStr"/>
+      <c r="BL4" t="inlineStr"/>
+      <c r="BM4" t="inlineStr"/>
+      <c r="BN4" t="inlineStr"/>
+      <c r="BO4" t="inlineStr"/>
+      <c r="BP4" t="inlineStr"/>
+      <c r="BQ4" t="inlineStr"/>
+      <c r="BR4" t="inlineStr"/>
+      <c r="BS4" t="inlineStr"/>
+      <c r="BT4" t="inlineStr"/>
+      <c r="BU4" t="inlineStr"/>
+      <c r="BV4" t="inlineStr"/>
+      <c r="BW4" t="inlineStr"/>
+      <c r="BX4" t="inlineStr"/>
+      <c r="BY4" t="inlineStr"/>
+      <c r="BZ4" t="inlineStr"/>
+      <c r="CA4" t="inlineStr"/>
+      <c r="CB4" t="inlineStr"/>
+      <c r="CC4" t="inlineStr"/>
+      <c r="CD4" t="inlineStr"/>
+      <c r="CE4" t="inlineStr"/>
+      <c r="CF4" t="inlineStr"/>
+      <c r="CG4" t="inlineStr"/>
+      <c r="CH4" t="inlineStr"/>
+      <c r="CI4" t="inlineStr"/>
+      <c r="CJ4" t="inlineStr"/>
+      <c r="CK4" t="inlineStr"/>
+      <c r="CL4" t="inlineStr"/>
+      <c r="CM4" t="inlineStr"/>
+      <c r="CN4" t="inlineStr"/>
+      <c r="CO4" t="inlineStr"/>
+      <c r="CP4" t="inlineStr"/>
+      <c r="CQ4" t="inlineStr"/>
+      <c r="CR4" t="inlineStr"/>
+      <c r="CS4" t="inlineStr"/>
+      <c r="CT4" t="inlineStr"/>
+      <c r="CU4" t="inlineStr"/>
+      <c r="CV4" t="inlineStr"/>
+      <c r="CW4" t="inlineStr"/>
+      <c r="CX4" t="inlineStr"/>
+      <c r="CY4" t="inlineStr"/>
+      <c r="CZ4" t="inlineStr"/>
+      <c r="DA4" t="inlineStr"/>
+      <c r="DB4" t="inlineStr"/>
+      <c r="DC4" t="inlineStr"/>
+      <c r="DD4" t="inlineStr"/>
+      <c r="DE4" t="inlineStr"/>
+      <c r="DF4" t="inlineStr"/>
+      <c r="DG4" t="inlineStr"/>
+      <c r="DH4" t="inlineStr"/>
+      <c r="DI4" t="inlineStr"/>
+      <c r="DJ4" t="inlineStr"/>
+      <c r="DK4" t="inlineStr"/>
+      <c r="DL4" t="inlineStr"/>
+      <c r="DM4" t="inlineStr"/>
+      <c r="DN4" t="inlineStr"/>
+      <c r="DO4" t="inlineStr"/>
+      <c r="DP4" t="inlineStr"/>
+      <c r="DQ4" t="inlineStr"/>
+      <c r="DR4" t="inlineStr"/>
+      <c r="DS4" t="inlineStr"/>
+      <c r="DT4" t="inlineStr"/>
+      <c r="DU4" t="inlineStr"/>
+      <c r="DV4" t="inlineStr"/>
+      <c r="DW4" t="inlineStr"/>
+      <c r="DX4" t="inlineStr"/>
+      <c r="DY4" t="inlineStr"/>
+      <c r="DZ4" t="inlineStr"/>
+      <c r="EA4" t="inlineStr"/>
+      <c r="EB4" t="inlineStr"/>
+      <c r="EC4" t="inlineStr"/>
+      <c r="ED4" t="inlineStr"/>
+      <c r="EE4" t="inlineStr"/>
+      <c r="EF4" t="inlineStr"/>
+      <c r="EG4" t="inlineStr"/>
+      <c r="EH4" t="inlineStr"/>
+      <c r="EI4" t="inlineStr"/>
+      <c r="EJ4" t="inlineStr"/>
+      <c r="EK4" t="inlineStr"/>
+      <c r="EL4" t="inlineStr"/>
+      <c r="EM4" t="inlineStr"/>
+      <c r="EN4" t="inlineStr"/>
+      <c r="EO4" t="inlineStr"/>
+      <c r="EP4" t="inlineStr"/>
+      <c r="EQ4" t="inlineStr"/>
+      <c r="ER4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
+          <t>hk</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>1</v>
+      </c>
+      <c r="C5" t="n">
+        <v>1</v>
+      </c>
+      <c r="D5" t="n">
+        <v>1</v>
+      </c>
+      <c r="E5" t="n">
+        <v>1</v>
+      </c>
+      <c r="F5" t="n">
+        <v>1</v>
+      </c>
+      <c r="G5" t="n">
+        <v>5</v>
+      </c>
+      <c r="H5" t="n">
+        <v>1</v>
+      </c>
+      <c r="I5" t="n">
+        <v>1</v>
+      </c>
+      <c r="J5" t="n">
+        <v>1</v>
+      </c>
+      <c r="K5" t="n">
+        <v>1</v>
+      </c>
+      <c r="L5" t="n">
+        <v>1</v>
+      </c>
+      <c r="M5" t="n">
+        <v>1</v>
+      </c>
+      <c r="N5" t="n">
+        <v>1</v>
+      </c>
+      <c r="O5" t="n">
+        <v>10</v>
+      </c>
+      <c r="P5" t="n">
+        <v>1</v>
+      </c>
+      <c r="Q5" t="n">
+        <v>1</v>
+      </c>
+      <c r="R5" t="n">
+        <v>1</v>
+      </c>
+      <c r="S5" t="n">
+        <v>1</v>
+      </c>
+      <c r="T5" t="n">
+        <v>1</v>
+      </c>
+      <c r="U5" t="n">
+        <v>1</v>
+      </c>
+      <c r="V5" t="n">
+        <v>2</v>
+      </c>
+      <c r="W5" t="n">
+        <v>1</v>
+      </c>
+      <c r="X5" t="n">
+        <v>16</v>
+      </c>
+      <c r="Y5" t="n">
+        <v>1</v>
+      </c>
+      <c r="Z5" t="n">
+        <v>1</v>
+      </c>
+      <c r="AA5" t="n">
+        <v>1</v>
+      </c>
+      <c r="AB5" t="n">
+        <v>2</v>
+      </c>
+      <c r="AC5" t="n">
+        <v>1</v>
+      </c>
+      <c r="AD5" t="n">
+        <v>1</v>
+      </c>
+      <c r="AE5" t="n">
+        <v>1</v>
+      </c>
+      <c r="AF5" t="n">
+        <v>1</v>
+      </c>
+      <c r="AG5" t="n">
+        <v>1</v>
+      </c>
+      <c r="AH5" t="n">
+        <v>1</v>
+      </c>
+      <c r="AI5" t="n">
+        <v>1</v>
+      </c>
+      <c r="AJ5" t="n">
+        <v>1</v>
+      </c>
+      <c r="AK5" t="n">
+        <v>1</v>
+      </c>
+      <c r="AL5" t="n">
+        <v>1</v>
+      </c>
+      <c r="AM5" t="n">
+        <v>1</v>
+      </c>
+      <c r="AN5" t="n">
+        <v>1</v>
+      </c>
+      <c r="AO5" t="n">
+        <v>1</v>
+      </c>
+      <c r="AP5" t="n">
+        <v>1</v>
+      </c>
+      <c r="AQ5" t="n">
+        <v>1</v>
+      </c>
+      <c r="AR5" t="n">
+        <v>1</v>
+      </c>
+      <c r="AS5" t="n">
+        <v>1</v>
+      </c>
+      <c r="AT5" t="n">
+        <v>2</v>
+      </c>
+      <c r="AU5" t="n">
+        <v>1</v>
+      </c>
+      <c r="AV5" t="n">
+        <v>3</v>
+      </c>
+      <c r="AW5" t="n">
+        <v>1</v>
+      </c>
+      <c r="AX5" t="n">
+        <v>3</v>
+      </c>
+      <c r="AY5" t="n">
+        <v>1</v>
+      </c>
+      <c r="AZ5" t="n">
+        <v>1</v>
+      </c>
+      <c r="BA5" t="n">
+        <v>1</v>
+      </c>
+      <c r="BB5" t="n">
+        <v>1</v>
+      </c>
+      <c r="BC5" t="n">
+        <v>1</v>
+      </c>
+      <c r="BD5" t="n">
+        <v>1</v>
+      </c>
+      <c r="BE5" t="n">
+        <v>1</v>
+      </c>
+      <c r="BF5" t="n">
+        <v>1</v>
+      </c>
+      <c r="BG5" t="n">
+        <v>1</v>
+      </c>
+      <c r="BH5" t="n">
+        <v>1</v>
+      </c>
+      <c r="BI5" t="n">
+        <v>2</v>
+      </c>
+      <c r="BJ5" t="n">
+        <v>1</v>
+      </c>
+      <c r="BK5" t="n">
+        <v>1</v>
+      </c>
+      <c r="BL5" t="n">
+        <v>1</v>
+      </c>
+      <c r="BM5" t="n">
+        <v>2</v>
+      </c>
+      <c r="BN5" t="n">
+        <v>1</v>
+      </c>
+      <c r="BO5" t="n">
+        <v>1</v>
+      </c>
+      <c r="BP5" t="n">
+        <v>5</v>
+      </c>
+      <c r="BQ5" t="n">
+        <v>1</v>
+      </c>
+      <c r="BR5" t="n">
+        <v>5</v>
+      </c>
+      <c r="BS5" t="n">
+        <v>1</v>
+      </c>
+      <c r="BT5" t="n">
+        <v>1</v>
+      </c>
+      <c r="BU5" t="n">
+        <v>1</v>
+      </c>
+      <c r="BV5" t="n">
+        <v>1</v>
+      </c>
+      <c r="BW5" t="n">
+        <v>1</v>
+      </c>
+      <c r="BX5" t="n">
+        <v>1</v>
+      </c>
+      <c r="BY5" t="n">
+        <v>1</v>
+      </c>
+      <c r="BZ5" t="n">
+        <v>1</v>
+      </c>
+      <c r="CA5" t="n">
+        <v>1</v>
+      </c>
+      <c r="CB5" t="n">
+        <v>1</v>
+      </c>
+      <c r="CC5" t="n">
+        <v>1</v>
+      </c>
+      <c r="CD5" t="n">
+        <v>1</v>
+      </c>
+      <c r="CE5" t="n">
+        <v>1</v>
+      </c>
+      <c r="CF5" t="n">
+        <v>1</v>
+      </c>
+      <c r="CG5" t="n">
+        <v>1</v>
+      </c>
+      <c r="CH5" t="n">
+        <v>1</v>
+      </c>
+      <c r="CI5" t="n">
+        <v>1</v>
+      </c>
+      <c r="CJ5" t="n">
+        <v>1</v>
+      </c>
+      <c r="CK5" t="n">
+        <v>1</v>
+      </c>
+      <c r="CL5" t="n">
+        <v>1</v>
+      </c>
+      <c r="CM5" t="n">
+        <v>1</v>
+      </c>
+      <c r="CN5" t="n">
+        <v>1</v>
+      </c>
+      <c r="CO5" t="n">
+        <v>1</v>
+      </c>
+      <c r="CP5" t="n">
+        <v>1</v>
+      </c>
+      <c r="CQ5" t="n">
+        <v>1</v>
+      </c>
+      <c r="CR5" t="n">
+        <v>1</v>
+      </c>
+      <c r="CS5" t="n">
+        <v>1</v>
+      </c>
+      <c r="CT5" t="n">
+        <v>1</v>
+      </c>
+      <c r="CU5" t="n">
+        <v>1</v>
+      </c>
+      <c r="CV5" t="n">
+        <v>1</v>
+      </c>
+      <c r="CW5" t="n">
+        <v>1</v>
+      </c>
+      <c r="CX5" t="n">
+        <v>1</v>
+      </c>
+      <c r="CY5" t="n">
+        <v>2</v>
+      </c>
+      <c r="CZ5" t="n">
+        <v>2</v>
+      </c>
+      <c r="DA5" t="n">
+        <v>2</v>
+      </c>
+      <c r="DB5" t="n">
+        <v>1</v>
+      </c>
+      <c r="DC5" t="n">
+        <v>1</v>
+      </c>
+      <c r="DD5" t="n">
+        <v>1</v>
+      </c>
+      <c r="DE5" t="n">
+        <v>1</v>
+      </c>
+      <c r="DF5" t="n">
+        <v>1</v>
+      </c>
+      <c r="DG5" t="n">
+        <v>1</v>
+      </c>
+      <c r="DH5" t="n">
+        <v>1</v>
+      </c>
+      <c r="DI5" t="n">
+        <v>4</v>
+      </c>
+      <c r="DJ5" t="n">
+        <v>1</v>
+      </c>
+      <c r="DK5" t="n">
+        <v>1</v>
+      </c>
+      <c r="DL5" t="n">
+        <v>6</v>
+      </c>
+      <c r="DM5" t="n">
+        <v>1</v>
+      </c>
+      <c r="DN5" t="n">
+        <v>3</v>
+      </c>
+      <c r="DO5" t="n">
+        <v>1</v>
+      </c>
+      <c r="DP5" t="n">
+        <v>1</v>
+      </c>
+      <c r="DQ5" t="n">
+        <v>1</v>
+      </c>
+      <c r="DR5" t="n">
+        <v>2</v>
+      </c>
+      <c r="DS5" t="n">
+        <v>1</v>
+      </c>
+      <c r="DT5" t="n">
+        <v>1</v>
+      </c>
+      <c r="DU5" t="n">
+        <v>1</v>
+      </c>
+      <c r="DV5" t="n">
+        <v>1</v>
+      </c>
+      <c r="DW5" t="n">
+        <v>4</v>
+      </c>
+      <c r="DX5" t="n">
+        <v>1</v>
+      </c>
+      <c r="DY5" t="n">
+        <v>1</v>
+      </c>
+      <c r="DZ5" t="n">
+        <v>1</v>
+      </c>
+      <c r="EA5" t="n">
+        <v>1</v>
+      </c>
+      <c r="EB5" t="n">
+        <v>1</v>
+      </c>
+      <c r="EC5" t="n">
+        <v>1</v>
+      </c>
+      <c r="ED5" t="n">
+        <v>1</v>
+      </c>
+      <c r="EE5" t="n">
+        <v>1</v>
+      </c>
+      <c r="EF5" t="n">
+        <v>1</v>
+      </c>
+      <c r="EG5" t="n">
+        <v>1</v>
+      </c>
+      <c r="EH5" t="n">
+        <v>1</v>
+      </c>
+      <c r="EI5" t="n">
+        <v>1</v>
+      </c>
+      <c r="EJ5" t="n">
+        <v>2</v>
+      </c>
+      <c r="EK5" t="n">
+        <v>1</v>
+      </c>
+      <c r="EL5" t="n">
+        <v>1</v>
+      </c>
+      <c r="EM5" t="n">
+        <v>1</v>
+      </c>
+      <c r="EN5" t="n">
+        <v>6</v>
+      </c>
+      <c r="EO5" t="n">
+        <v>2</v>
+      </c>
+      <c r="EP5" t="n">
+        <v>1</v>
+      </c>
+      <c r="EQ5" t="n">
+        <v>1</v>
+      </c>
+      <c r="ER5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
           <t>λk</t>
         </is>
       </c>
-      <c r="B5" t="n">
+      <c r="B6" t="n">
         <v>-2</v>
       </c>
-      <c r="C5" t="n">
+      <c r="C6" t="n">
         <v>-5</v>
       </c>
-      <c r="D5" t="n">
+      <c r="D6" t="n">
         <v>-4</v>
       </c>
-      <c r="E5" t="n">
+      <c r="E6" t="n">
         <v>-3</v>
       </c>
-      <c r="F5" t="n">
+      <c r="F6" t="n">
         <v>-2</v>
       </c>
-      <c r="G5" t="n">
+      <c r="G6" t="n">
         <v>-1</v>
       </c>
-      <c r="H5" t="n">
-        <v>0</v>
-      </c>
-      <c r="I5" t="n">
-        <v>0</v>
-      </c>
-      <c r="J5" t="n">
+      <c r="H6" t="n">
+        <v>0</v>
+      </c>
+      <c r="I6" t="n">
+        <v>0</v>
+      </c>
+      <c r="J6" t="n">
         <v>-4</v>
       </c>
-      <c r="K5" t="n">
+      <c r="K6" t="n">
         <v>-4</v>
       </c>
-      <c r="L5" t="n">
+      <c r="L6" t="n">
         <v>-3</v>
       </c>
-      <c r="M5" t="n">
+      <c r="M6" t="n">
         <v>-2</v>
       </c>
-      <c r="N5" t="n">
+      <c r="N6" t="n">
         <v>-2</v>
       </c>
-      <c r="O5" t="n">
+      <c r="O6" t="n">
         <v>-1</v>
       </c>
-      <c r="P5" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q5" t="n">
+      <c r="P6" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q6" t="n">
         <v>-1</v>
       </c>
-      <c r="R5" t="n">
-        <v>0</v>
-      </c>
-      <c r="S5" t="n">
-        <v>0</v>
-      </c>
-      <c r="T5" t="n">
+      <c r="R6" t="n">
+        <v>0</v>
+      </c>
+      <c r="S6" t="n">
+        <v>0</v>
+      </c>
+      <c r="T6" t="n">
         <v>-2</v>
       </c>
-      <c r="U5" t="n">
-        <v>0</v>
-      </c>
-      <c r="V5" t="n">
-        <v>0</v>
-      </c>
-      <c r="W5" t="n">
+      <c r="U6" t="n">
+        <v>0</v>
+      </c>
+      <c r="V6" t="n">
+        <v>0</v>
+      </c>
+      <c r="W6" t="n">
         <v>-1</v>
       </c>
-      <c r="X5" t="n">
-        <v>0</v>
-      </c>
-      <c r="Y5" t="n">
-        <v>1</v>
-      </c>
-      <c r="Z5" t="n">
-        <v>1</v>
-      </c>
-      <c r="AA5" t="n">
+      <c r="X6" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y6" t="n">
+        <v>1</v>
+      </c>
+      <c r="Z6" t="n">
+        <v>1</v>
+      </c>
+      <c r="AA6" t="n">
         <v>-1</v>
       </c>
-      <c r="AB5" t="n">
-        <v>0</v>
-      </c>
-      <c r="AC5" t="n">
+      <c r="AB6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AC6" t="n">
         <v>6</v>
       </c>
-      <c r="AD5" t="n">
+      <c r="AD6" t="n">
         <v>-8</v>
       </c>
-      <c r="AE5" t="n">
+      <c r="AE6" t="n">
         <v>-1</v>
       </c>
-      <c r="AF5" t="n">
-        <v>0</v>
-      </c>
-      <c r="AG5" t="n">
+      <c r="AF6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AG6" t="n">
         <v>-1</v>
       </c>
-      <c r="AH5" t="n">
-        <v>0</v>
-      </c>
-      <c r="AI5" t="n">
-        <v>0</v>
-      </c>
-      <c r="AJ5" t="n">
+      <c r="AH6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AI6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ6" t="n">
         <v>-1</v>
       </c>
-      <c r="AK5" t="n">
+      <c r="AK6" t="n">
         <v>6</v>
       </c>
-      <c r="AL5" t="n">
+      <c r="AL6" t="n">
         <v>-6</v>
       </c>
-      <c r="AM5" t="n">
+      <c r="AM6" t="n">
         <v>-1</v>
       </c>
-      <c r="AN5" t="n">
+      <c r="AN6" t="n">
         <v>6</v>
       </c>
-      <c r="AO5" t="n">
+      <c r="AO6" t="n">
         <v>-1</v>
       </c>
-      <c r="AP5" t="n">
+      <c r="AP6" t="n">
         <v>-5</v>
       </c>
-      <c r="AQ5" t="n">
+      <c r="AQ6" t="n">
         <v>-1</v>
       </c>
-      <c r="AR5" t="n">
+      <c r="AR6" t="n">
         <v>6</v>
       </c>
-      <c r="AS5" t="n">
+      <c r="AS6" t="n">
         <v>-1</v>
       </c>
-      <c r="AT5" t="n">
+      <c r="AT6" t="n">
         <v>-2.5</v>
       </c>
-      <c r="AU5" t="n">
+      <c r="AU6" t="n">
         <v>-1</v>
       </c>
-      <c r="AV5" t="n">
+      <c r="AV6" t="n">
         <v>2</v>
       </c>
-      <c r="AW5" t="n">
+      <c r="AW6" t="n">
         <v>-1</v>
       </c>
-      <c r="AX5" t="n">
+      <c r="AX6" t="n">
         <v>-1.666666666666667</v>
       </c>
-      <c r="AY5" t="n">
+      <c r="AY6" t="n">
         <v>-1</v>
       </c>
-      <c r="AZ5" t="n">
+      <c r="AZ6" t="n">
         <v>-1</v>
       </c>
-      <c r="BA5" t="n">
-        <v>0</v>
-      </c>
-      <c r="BB5" t="n">
-        <v>0</v>
-      </c>
-      <c r="BC5" t="n">
+      <c r="BA6" t="n">
+        <v>0</v>
+      </c>
+      <c r="BB6" t="n">
+        <v>0</v>
+      </c>
+      <c r="BC6" t="n">
         <v>-2</v>
       </c>
-      <c r="BD5" t="n">
-        <v>0</v>
-      </c>
-      <c r="BE5" t="n">
+      <c r="BD6" t="n">
+        <v>0</v>
+      </c>
+      <c r="BE6" t="n">
         <v>-3</v>
       </c>
-      <c r="BF5" t="n">
+      <c r="BF6" t="n">
         <v>-3</v>
       </c>
-      <c r="BG5" t="n">
+      <c r="BG6" t="n">
         <v>-2</v>
       </c>
-      <c r="BH5" t="n">
+      <c r="BH6" t="n">
         <v>-3</v>
       </c>
-      <c r="BI5" t="n">
+      <c r="BI6" t="n">
         <v>-1.5</v>
       </c>
-      <c r="BJ5" t="n">
+      <c r="BJ6" t="n">
         <v>-1</v>
       </c>
-      <c r="BK5" t="n">
-        <v>0</v>
-      </c>
-      <c r="BL5" t="n">
+      <c r="BK6" t="n">
+        <v>0</v>
+      </c>
+      <c r="BL6" t="n">
         <v>-1</v>
       </c>
-      <c r="BM5" t="n">
-        <v>0</v>
-      </c>
-      <c r="BN5" t="n">
+      <c r="BM6" t="n">
+        <v>0</v>
+      </c>
+      <c r="BN6" t="n">
         <v>-1</v>
       </c>
-      <c r="BO5" t="n">
-        <v>0</v>
-      </c>
-      <c r="BP5" t="n">
-        <v>0</v>
-      </c>
-      <c r="BQ5" t="n">
+      <c r="BO6" t="n">
+        <v>0</v>
+      </c>
+      <c r="BP6" t="n">
+        <v>0</v>
+      </c>
+      <c r="BQ6" t="n">
         <v>-1</v>
       </c>
-      <c r="BR5" t="n">
-        <v>0</v>
-      </c>
-      <c r="BS5" t="n">
+      <c r="BR6" t="n">
+        <v>0</v>
+      </c>
+      <c r="BS6" t="n">
         <v>-1</v>
       </c>
-      <c r="BT5" t="n">
+      <c r="BT6" t="n">
         <v>2</v>
       </c>
-      <c r="BU5" t="n">
-        <v>1</v>
-      </c>
-      <c r="BV5" t="n">
-        <v>0</v>
-      </c>
-      <c r="BW5" t="n">
-        <v>0</v>
-      </c>
-      <c r="BX5" t="n">
-        <v>1</v>
-      </c>
-      <c r="BY5" t="n">
-        <v>1</v>
-      </c>
-      <c r="BZ5" t="n">
-        <v>0</v>
-      </c>
-      <c r="CA5" t="n">
-        <v>0</v>
-      </c>
-      <c r="CB5" t="n">
+      <c r="BU6" t="n">
+        <v>1</v>
+      </c>
+      <c r="BV6" t="n">
+        <v>0</v>
+      </c>
+      <c r="BW6" t="n">
+        <v>0</v>
+      </c>
+      <c r="BX6" t="n">
+        <v>1</v>
+      </c>
+      <c r="BY6" t="n">
+        <v>1</v>
+      </c>
+      <c r="BZ6" t="n">
+        <v>0</v>
+      </c>
+      <c r="CA6" t="n">
+        <v>0</v>
+      </c>
+      <c r="CB6" t="n">
         <v>23</v>
       </c>
-      <c r="CC5" t="n">
+      <c r="CC6" t="n">
         <v>8</v>
       </c>
-      <c r="CD5" t="n">
+      <c r="CD6" t="n">
         <v>-11</v>
       </c>
-      <c r="CE5" t="n">
+      <c r="CE6" t="n">
         <v>12</v>
       </c>
-      <c r="CF5" t="n">
+      <c r="CF6" t="n">
         <v>-27</v>
       </c>
-      <c r="CG5" t="n">
+      <c r="CG6" t="n">
         <v>2</v>
       </c>
-      <c r="CH5" t="n">
+      <c r="CH6" t="n">
         <v>24</v>
       </c>
-      <c r="CI5" t="n">
+      <c r="CI6" t="n">
         <v>4</v>
       </c>
-      <c r="CJ5" t="n">
-        <v>1</v>
-      </c>
-      <c r="CK5" t="n">
+      <c r="CJ6" t="n">
+        <v>1</v>
+      </c>
+      <c r="CK6" t="n">
         <v>4</v>
       </c>
-      <c r="CL5" t="n">
+      <c r="CL6" t="n">
         <v>-9</v>
       </c>
-      <c r="CM5" t="n">
-        <v>1</v>
-      </c>
-      <c r="CN5" t="n">
-        <v>0</v>
-      </c>
-      <c r="CO5" t="n">
-        <v>3</v>
-      </c>
-      <c r="CP5" t="n">
+      <c r="CM6" t="n">
+        <v>1</v>
+      </c>
+      <c r="CN6" t="n">
+        <v>0</v>
+      </c>
+      <c r="CO6" t="n">
+        <v>3</v>
+      </c>
+      <c r="CP6" t="n">
         <v>-1</v>
       </c>
-      <c r="CQ5" t="n">
+      <c r="CQ6" t="n">
         <v>4</v>
       </c>
-      <c r="CR5" t="n">
+      <c r="CR6" t="n">
         <v>-4</v>
       </c>
-      <c r="CS5" t="n">
-        <v>1</v>
-      </c>
-      <c r="CT5" t="n">
-        <v>0</v>
-      </c>
-      <c r="CU5" t="n">
-        <v>0</v>
-      </c>
-      <c r="CV5" t="n">
+      <c r="CS6" t="n">
+        <v>1</v>
+      </c>
+      <c r="CT6" t="n">
+        <v>0</v>
+      </c>
+      <c r="CU6" t="n">
+        <v>0</v>
+      </c>
+      <c r="CV6" t="n">
         <v>2</v>
       </c>
-      <c r="CW5" t="n">
-        <v>0</v>
-      </c>
-      <c r="CX5" t="n">
-        <v>0</v>
-      </c>
-      <c r="CY5" t="n">
-        <v>1</v>
-      </c>
-      <c r="CZ5" t="n">
+      <c r="CW6" t="n">
+        <v>0</v>
+      </c>
+      <c r="CX6" t="n">
+        <v>0</v>
+      </c>
+      <c r="CY6" t="n">
+        <v>1</v>
+      </c>
+      <c r="CZ6" t="n">
         <v>1.5</v>
       </c>
-      <c r="DA5" t="n">
+      <c r="DA6" t="n">
         <v>1.5</v>
       </c>
-      <c r="DB5" t="n">
+      <c r="DB6" t="n">
         <v>2</v>
       </c>
-      <c r="DC5" t="n">
+      <c r="DC6" t="n">
         <v>2</v>
       </c>
-      <c r="DD5" t="n">
+      <c r="DD6" t="n">
         <v>2</v>
       </c>
-      <c r="DE5" t="n">
+      <c r="DE6" t="n">
         <v>4</v>
       </c>
-      <c r="DF5" t="n">
+      <c r="DF6" t="n">
         <v>14</v>
       </c>
-      <c r="DG5" t="n">
-        <v>0</v>
-      </c>
-      <c r="DH5" t="n">
+      <c r="DG6" t="n">
+        <v>0</v>
+      </c>
+      <c r="DH6" t="n">
         <v>2</v>
       </c>
-      <c r="DI5" t="n">
+      <c r="DI6" t="n">
         <v>1.5</v>
       </c>
-      <c r="DJ5" t="n">
-        <v>3</v>
-      </c>
-      <c r="DK5" t="n">
-        <v>0</v>
-      </c>
-      <c r="DL5" t="n">
-        <v>0</v>
-      </c>
-      <c r="DM5" t="n">
-        <v>1</v>
-      </c>
-      <c r="DN5" t="n">
-        <v>0</v>
-      </c>
-      <c r="DO5" t="n">
-        <v>1</v>
-      </c>
-      <c r="DP5" t="n">
+      <c r="DJ6" t="n">
+        <v>3</v>
+      </c>
+      <c r="DK6" t="n">
+        <v>0</v>
+      </c>
+      <c r="DL6" t="n">
+        <v>0</v>
+      </c>
+      <c r="DM6" t="n">
+        <v>1</v>
+      </c>
+      <c r="DN6" t="n">
+        <v>0</v>
+      </c>
+      <c r="DO6" t="n">
+        <v>1</v>
+      </c>
+      <c r="DP6" t="n">
         <v>8</v>
       </c>
-      <c r="DQ5" t="n">
+      <c r="DQ6" t="n">
         <v>-8</v>
       </c>
-      <c r="DR5" t="n">
-        <v>0</v>
-      </c>
-      <c r="DS5" t="n">
+      <c r="DR6" t="n">
+        <v>0</v>
+      </c>
+      <c r="DS6" t="n">
         <v>-3</v>
       </c>
-      <c r="DT5" t="n">
-        <v>0</v>
-      </c>
-      <c r="DU5" t="n">
+      <c r="DT6" t="n">
+        <v>0</v>
+      </c>
+      <c r="DU6" t="n">
         <v>-1</v>
       </c>
-      <c r="DV5" t="n">
-        <v>0</v>
-      </c>
-      <c r="DW5" t="n">
-        <v>0</v>
-      </c>
-      <c r="DX5" t="n">
-        <v>0</v>
-      </c>
-      <c r="DY5" t="n">
-        <v>1</v>
-      </c>
-      <c r="DZ5" t="n">
-        <v>0</v>
-      </c>
-      <c r="EA5" t="n">
-        <v>3</v>
-      </c>
-      <c r="EB5" t="n">
-        <v>0</v>
-      </c>
-      <c r="EC5" t="n">
-        <v>0</v>
-      </c>
-      <c r="ED5" t="n">
+      <c r="DV6" t="n">
+        <v>0</v>
+      </c>
+      <c r="DW6" t="n">
+        <v>0</v>
+      </c>
+      <c r="DX6" t="n">
+        <v>0</v>
+      </c>
+      <c r="DY6" t="n">
+        <v>1</v>
+      </c>
+      <c r="DZ6" t="n">
+        <v>0</v>
+      </c>
+      <c r="EA6" t="n">
+        <v>3</v>
+      </c>
+      <c r="EB6" t="n">
+        <v>0</v>
+      </c>
+      <c r="EC6" t="n">
+        <v>0</v>
+      </c>
+      <c r="ED6" t="n">
         <v>-1</v>
       </c>
-      <c r="EE5" t="n">
-        <v>0</v>
-      </c>
-      <c r="EF5" t="n">
-        <v>1</v>
-      </c>
-      <c r="EG5" t="n">
-        <v>0</v>
-      </c>
-      <c r="EH5" t="n">
-        <v>0</v>
-      </c>
-      <c r="EI5" t="n">
+      <c r="EE6" t="n">
+        <v>0</v>
+      </c>
+      <c r="EF6" t="n">
+        <v>1</v>
+      </c>
+      <c r="EG6" t="n">
+        <v>0</v>
+      </c>
+      <c r="EH6" t="n">
+        <v>0</v>
+      </c>
+      <c r="EI6" t="n">
         <v>-1</v>
       </c>
-      <c r="EJ5" t="n">
-        <v>0</v>
-      </c>
-      <c r="EK5" t="n">
-        <v>0</v>
-      </c>
-      <c r="EL5" t="n">
-        <v>1</v>
-      </c>
-      <c r="EM5" t="n">
-        <v>0</v>
-      </c>
-      <c r="EN5" t="n">
-        <v>1</v>
-      </c>
-      <c r="EO5" t="n">
+      <c r="EJ6" t="n">
+        <v>0</v>
+      </c>
+      <c r="EK6" t="n">
+        <v>0</v>
+      </c>
+      <c r="EL6" t="n">
+        <v>1</v>
+      </c>
+      <c r="EM6" t="n">
+        <v>0</v>
+      </c>
+      <c r="EN6" t="n">
+        <v>1</v>
+      </c>
+      <c r="EO6" t="n">
         <v>2</v>
       </c>
-      <c r="EP5" t="n">
-        <v>0</v>
-      </c>
-      <c r="EQ5" t="n">
-        <v>0</v>
-      </c>
-      <c r="ER5" t="n">
+      <c r="EP6" t="n">
+        <v>0</v>
+      </c>
+      <c r="EQ6" t="n">
+        <v>0</v>
+      </c>
+      <c r="ER6" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>μk</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>0</v>
+      </c>
+      <c r="C7" t="n">
+        <v>-9</v>
+      </c>
+      <c r="D7" t="n">
+        <v>3</v>
+      </c>
+      <c r="E7" t="n">
+        <v>3</v>
+      </c>
+      <c r="F7" t="n">
+        <v>3</v>
+      </c>
+      <c r="G7" t="n">
+        <v>3</v>
+      </c>
+      <c r="H7" t="n">
+        <v>3</v>
+      </c>
+      <c r="I7" t="n">
+        <v>0</v>
+      </c>
+      <c r="J7" t="n">
+        <v>-12</v>
+      </c>
+      <c r="K7" t="n">
+        <v>0</v>
+      </c>
+      <c r="L7" t="n">
+        <v>3</v>
+      </c>
+      <c r="M7" t="n">
+        <v>3</v>
+      </c>
+      <c r="N7" t="n">
+        <v>0</v>
+      </c>
+      <c r="O7" t="n">
+        <v>3</v>
+      </c>
+      <c r="P7" t="n">
+        <v>3</v>
+      </c>
+      <c r="Q7" t="n">
+        <v>-3</v>
+      </c>
+      <c r="R7" t="n">
+        <v>3</v>
+      </c>
+      <c r="S7" t="n">
+        <v>0</v>
+      </c>
+      <c r="T7" t="n">
+        <v>-6</v>
+      </c>
+      <c r="U7" t="n">
+        <v>6</v>
+      </c>
+      <c r="V7" t="n">
+        <v>0</v>
+      </c>
+      <c r="W7" t="n">
+        <v>-3</v>
+      </c>
+      <c r="X7" t="n">
+        <v>3</v>
+      </c>
+      <c r="Y7" t="n">
+        <v>3</v>
+      </c>
+      <c r="Z7" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA7" t="n">
+        <v>-6</v>
+      </c>
+      <c r="AB7" t="n">
+        <v>3</v>
+      </c>
+      <c r="AC7" t="n">
+        <v>18</v>
+      </c>
+      <c r="AD7" t="n">
+        <v>-42</v>
+      </c>
+      <c r="AE7" t="n">
+        <v>21</v>
+      </c>
+      <c r="AF7" t="n">
+        <v>3</v>
+      </c>
+      <c r="AG7" t="n">
+        <v>-3</v>
+      </c>
+      <c r="AH7" t="n">
+        <v>3</v>
+      </c>
+      <c r="AI7" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ7" t="n">
+        <v>-3</v>
+      </c>
+      <c r="AK7" t="n">
+        <v>21</v>
+      </c>
+      <c r="AL7" t="n">
+        <v>-36</v>
+      </c>
+      <c r="AM7" t="n">
+        <v>15</v>
+      </c>
+      <c r="AN7" t="n">
+        <v>21</v>
+      </c>
+      <c r="AO7" t="n">
+        <v>-21</v>
+      </c>
+      <c r="AP7" t="n">
+        <v>-12</v>
+      </c>
+      <c r="AQ7" t="n">
+        <v>12</v>
+      </c>
+      <c r="AR7" t="n">
+        <v>21</v>
+      </c>
+      <c r="AS7" t="n">
+        <v>-21</v>
+      </c>
+      <c r="AT7" t="n">
+        <v>-4.5</v>
+      </c>
+      <c r="AU7" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="AV7" t="n">
+        <v>9</v>
+      </c>
+      <c r="AW7" t="n">
+        <v>-9</v>
+      </c>
+      <c r="AX7" t="n">
+        <v>-2</v>
+      </c>
+      <c r="AY7" t="n">
+        <v>2</v>
+      </c>
+      <c r="AZ7" t="n">
+        <v>0</v>
+      </c>
+      <c r="BA7" t="n">
+        <v>3</v>
+      </c>
+      <c r="BB7" t="n">
+        <v>0</v>
+      </c>
+      <c r="BC7" t="n">
+        <v>-6</v>
+      </c>
+      <c r="BD7" t="n">
+        <v>6</v>
+      </c>
+      <c r="BE7" t="n">
+        <v>-9</v>
+      </c>
+      <c r="BF7" t="n">
+        <v>0</v>
+      </c>
+      <c r="BG7" t="n">
+        <v>3</v>
+      </c>
+      <c r="BH7" t="n">
+        <v>-3</v>
+      </c>
+      <c r="BI7" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="BJ7" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="BK7" t="n">
+        <v>3</v>
+      </c>
+      <c r="BL7" t="n">
+        <v>-3</v>
+      </c>
+      <c r="BM7" t="n">
+        <v>3</v>
+      </c>
+      <c r="BN7" t="n">
+        <v>-3</v>
+      </c>
+      <c r="BO7" t="n">
+        <v>3</v>
+      </c>
+      <c r="BP7" t="n">
+        <v>0</v>
+      </c>
+      <c r="BQ7" t="n">
+        <v>-3</v>
+      </c>
+      <c r="BR7" t="n">
+        <v>3</v>
+      </c>
+      <c r="BS7" t="n">
+        <v>-3</v>
+      </c>
+      <c r="BT7" t="n">
+        <v>9</v>
+      </c>
+      <c r="BU7" t="n">
+        <v>-3</v>
+      </c>
+      <c r="BV7" t="n">
+        <v>-3</v>
+      </c>
+      <c r="BW7" t="n">
+        <v>0</v>
+      </c>
+      <c r="BX7" t="n">
+        <v>3</v>
+      </c>
+      <c r="BY7" t="n">
+        <v>0</v>
+      </c>
+      <c r="BZ7" t="n">
+        <v>-3</v>
+      </c>
+      <c r="CA7" t="n">
+        <v>0</v>
+      </c>
+      <c r="CB7" t="n">
+        <v>69</v>
+      </c>
+      <c r="CC7" t="n">
+        <v>-45</v>
+      </c>
+      <c r="CD7" t="n">
+        <v>-57</v>
+      </c>
+      <c r="CE7" t="n">
+        <v>69</v>
+      </c>
+      <c r="CF7" t="n">
+        <v>-117</v>
+      </c>
+      <c r="CG7" t="n">
+        <v>87</v>
+      </c>
+      <c r="CH7" t="n">
+        <v>66</v>
+      </c>
+      <c r="CI7" t="n">
+        <v>-60</v>
+      </c>
+      <c r="CJ7" t="n">
+        <v>-9</v>
+      </c>
+      <c r="CK7" t="n">
+        <v>9</v>
+      </c>
+      <c r="CL7" t="n">
+        <v>-39</v>
+      </c>
+      <c r="CM7" t="n">
+        <v>30</v>
+      </c>
+      <c r="CN7" t="n">
+        <v>-3</v>
+      </c>
+      <c r="CO7" t="n">
+        <v>9</v>
+      </c>
+      <c r="CP7" t="n">
+        <v>-12</v>
+      </c>
+      <c r="CQ7" t="n">
+        <v>15</v>
+      </c>
+      <c r="CR7" t="n">
+        <v>-24</v>
+      </c>
+      <c r="CS7" t="n">
+        <v>15</v>
+      </c>
+      <c r="CT7" t="n">
+        <v>-3</v>
+      </c>
+      <c r="CU7" t="n">
+        <v>0</v>
+      </c>
+      <c r="CV7" t="n">
+        <v>6</v>
+      </c>
+      <c r="CW7" t="n">
+        <v>-6</v>
+      </c>
+      <c r="CX7" t="n">
+        <v>0</v>
+      </c>
+      <c r="CY7" t="n">
+        <v>3</v>
+      </c>
+      <c r="CZ7" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="DA7" t="n">
+        <v>0</v>
+      </c>
+      <c r="DB7" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="DC7" t="n">
+        <v>0</v>
+      </c>
+      <c r="DD7" t="n">
+        <v>0</v>
+      </c>
+      <c r="DE7" t="n">
+        <v>6</v>
+      </c>
+      <c r="DF7" t="n">
+        <v>30</v>
+      </c>
+      <c r="DG7" t="n">
+        <v>-42</v>
+      </c>
+      <c r="DH7" t="n">
+        <v>6</v>
+      </c>
+      <c r="DI7" t="n">
+        <v>-1.5</v>
+      </c>
+      <c r="DJ7" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="DK7" t="n">
+        <v>-9</v>
+      </c>
+      <c r="DL7" t="n">
+        <v>0</v>
+      </c>
+      <c r="DM7" t="n">
+        <v>3</v>
+      </c>
+      <c r="DN7" t="n">
+        <v>-3</v>
+      </c>
+      <c r="DO7" t="n">
+        <v>3</v>
+      </c>
+      <c r="DP7" t="n">
+        <v>21</v>
+      </c>
+      <c r="DQ7" t="n">
+        <v>-48</v>
+      </c>
+      <c r="DR7" t="n">
+        <v>24</v>
+      </c>
+      <c r="DS7" t="n">
+        <v>-9</v>
+      </c>
+      <c r="DT7" t="n">
+        <v>9</v>
+      </c>
+      <c r="DU7" t="n">
+        <v>-3</v>
+      </c>
+      <c r="DV7" t="n">
+        <v>3</v>
+      </c>
+      <c r="DW7" t="n">
+        <v>0</v>
+      </c>
+      <c r="DX7" t="n">
+        <v>0</v>
+      </c>
+      <c r="DY7" t="n">
+        <v>3</v>
+      </c>
+      <c r="DZ7" t="n">
+        <v>-3</v>
+      </c>
+      <c r="EA7" t="n">
+        <v>9</v>
+      </c>
+      <c r="EB7" t="n">
+        <v>-9</v>
+      </c>
+      <c r="EC7" t="n">
+        <v>0</v>
+      </c>
+      <c r="ED7" t="n">
+        <v>-3</v>
+      </c>
+      <c r="EE7" t="n">
+        <v>3</v>
+      </c>
+      <c r="EF7" t="n">
+        <v>3</v>
+      </c>
+      <c r="EG7" t="n">
+        <v>-3</v>
+      </c>
+      <c r="EH7" t="n">
+        <v>0</v>
+      </c>
+      <c r="EI7" t="n">
+        <v>-3</v>
+      </c>
+      <c r="EJ7" t="n">
+        <v>3</v>
+      </c>
+      <c r="EK7" t="n">
+        <v>0</v>
+      </c>
+      <c r="EL7" t="n">
+        <v>3</v>
+      </c>
+      <c r="EM7" t="n">
+        <v>-3</v>
+      </c>
+      <c r="EN7" t="n">
+        <v>3</v>
+      </c>
+      <c r="EO7" t="n">
+        <v>3</v>
+      </c>
+      <c r="EP7" t="n">
+        <v>-6</v>
+      </c>
+      <c r="EQ7" t="n">
+        <v>0</v>
+      </c>
+      <c r="ER7" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Valores de C calculados
</commit_message>
<xml_diff>
--- a/matriz_puntos.xlsx
+++ b/matriz_puntos.xlsx
@@ -9,6 +9,8 @@
   <sheets>
     <sheet name="Coordenadas y Elementos" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="Spline Natural" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Resultante Spline Natural" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="Valores C - ResulSist " sheetId="4" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -67824,4 +67826,2232 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A146"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>-9</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>-12</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>-3</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>-6</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="n">
+        <v>-3</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="n">
+        <v>-6</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="n">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="n">
+        <v>-42</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="n">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="n">
+        <v>-3</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="n">
+        <v>-3</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="n">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="n">
+        <v>-36</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="n">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="n">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="n">
+        <v>-21</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="n">
+        <v>-12</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="n">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="n">
+        <v>-21</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="n">
+        <v>-4.5</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="n">
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="n">
+        <v>-9</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="n">
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="n">
+        <v>-6</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="n">
+        <v>-9</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="n">
+        <v>-3</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="n">
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="n">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="n">
+        <v>-3</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="n">
+        <v>-3</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="n">
+        <v>-3</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="n">
+        <v>-3</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="n">
+        <v>-3</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="n">
+        <v>-3</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="n">
+        <v>-3</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="n">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="n">
+        <v>-45</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="n">
+        <v>-57</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="n">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="n">
+        <v>-117</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="n">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="n">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="n">
+        <v>-60</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="n">
+        <v>-9</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="n">
+        <v>-39</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="n">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="n">
+        <v>-3</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="n">
+        <v>-12</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="n">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="n">
+        <v>-24</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="n">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="n">
+        <v>-3</v>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="n">
+        <v>-6</v>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="n">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" t="n">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" t="n">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" t="n">
+        <v>-42</v>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" t="n">
+        <v>-1.5</v>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" t="n">
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" t="n">
+        <v>-9</v>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" t="n">
+        <v>-3</v>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" t="n">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" t="n">
+        <v>-48</v>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" t="n">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" t="n">
+        <v>-9</v>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124" t="n">
+        <v>-3</v>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="126">
+      <c r="A126" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="127">
+      <c r="A127" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="128">
+      <c r="A128" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="129">
+      <c r="A129" t="n">
+        <v>-3</v>
+      </c>
+    </row>
+    <row r="130">
+      <c r="A130" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="131">
+      <c r="A131" t="n">
+        <v>-9</v>
+      </c>
+    </row>
+    <row r="132">
+      <c r="A132" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="133">
+      <c r="A133" t="n">
+        <v>-3</v>
+      </c>
+    </row>
+    <row r="134">
+      <c r="A134" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="135">
+      <c r="A135" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="136">
+      <c r="A136" t="n">
+        <v>-3</v>
+      </c>
+    </row>
+    <row r="137">
+      <c r="A137" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="138">
+      <c r="A138" t="n">
+        <v>-3</v>
+      </c>
+    </row>
+    <row r="139">
+      <c r="A139" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="140">
+      <c r="A140" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="141">
+      <c r="A141" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="142">
+      <c r="A142" t="n">
+        <v>-3</v>
+      </c>
+    </row>
+    <row r="143">
+      <c r="A143" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="144">
+      <c r="A144" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="145">
+      <c r="A145" t="n">
+        <v>-6</v>
+      </c>
+    </row>
+    <row r="146">
+      <c r="A146" t="n">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B146"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>c0</t>
+        </is>
+      </c>
+      <c r="B1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>c1</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>-2.583</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>c2</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>1.3321</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>c3</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>0.2544</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>c4</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>0.6501</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>c5</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>0.1453</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>c6</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>0.1213</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>c7</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>0.8177</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>c8</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>-3.3923</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>c9</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>0.7514</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>c10</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>0.3866</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>c11</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>0.7020999999999999</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>c12</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>-0.1951</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>c13</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>0.0784</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>c14</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
+        <v>0.1471</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>c15</t>
+        </is>
+      </c>
+      <c r="B16" t="n">
+        <v>-1.0199</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>c16</t>
+        </is>
+      </c>
+      <c r="B17" t="n">
+        <v>0.9326</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>c17</t>
+        </is>
+      </c>
+      <c r="B18" t="n">
+        <v>0.2894</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>c18</t>
+        </is>
+      </c>
+      <c r="B19" t="n">
+        <v>-2.0902</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>c19</t>
+        </is>
+      </c>
+      <c r="B20" t="n">
+        <v>2.0715</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>c20</t>
+        </is>
+      </c>
+      <c r="B21" t="n">
+        <v>-0.1958</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>c21</t>
+        </is>
+      </c>
+      <c r="B22" t="n">
+        <v>-0.4485</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>c22</t>
+        </is>
+      </c>
+      <c r="B23" t="n">
+        <v>0.0824</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>c23</t>
+        </is>
+      </c>
+      <c r="B24" t="n">
+        <v>0.0404</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>c24</t>
+        </is>
+      </c>
+      <c r="B25" t="n">
+        <v>0.3083</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>c25</t>
+        </is>
+      </c>
+      <c r="B26" t="n">
+        <v>-1.2738</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>c26</t>
+        </is>
+      </c>
+      <c r="B27" t="n">
+        <v>-1.2132</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>c27</t>
+        </is>
+      </c>
+      <c r="B28" t="n">
+        <v>5.7766</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>c28</t>
+        </is>
+      </c>
+      <c r="B29" t="n">
+        <v>-14.2332</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>c29</t>
+        </is>
+      </c>
+      <c r="B30" t="n">
+        <v>9.1564</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>c30</t>
+        </is>
+      </c>
+      <c r="B31" t="n">
+        <v>-1.3922</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>c31</t>
+        </is>
+      </c>
+      <c r="B32" t="n">
+        <v>-0.5876</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>c32</t>
+        </is>
+      </c>
+      <c r="B33" t="n">
+        <v>0.7426</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>c33</t>
+        </is>
+      </c>
+      <c r="B34" t="n">
+        <v>0.6172</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>c34</t>
+        </is>
+      </c>
+      <c r="B35" t="n">
+        <v>-3.2114</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>c35</t>
+        </is>
+      </c>
+      <c r="B36" t="n">
+        <v>9.228400000000001</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>c36</t>
+        </is>
+      </c>
+      <c r="B37" t="n">
+        <v>-12.702</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>c37</t>
+        </is>
+      </c>
+      <c r="B38" t="n">
+        <v>5.5797</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>c38</t>
+        </is>
+      </c>
+      <c r="B39" t="n">
+        <v>5.3831</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>c39</t>
+        </is>
+      </c>
+      <c r="B40" t="n">
+        <v>-6.112</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>c40</t>
+        </is>
+      </c>
+      <c r="B41" t="n">
+        <v>-1.9351</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>c41</t>
+        </is>
+      </c>
+      <c r="B42" t="n">
+        <v>1.8525</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>c42</t>
+        </is>
+      </c>
+      <c r="B43" t="n">
+        <v>6.5252</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>c43</t>
+        </is>
+      </c>
+      <c r="B44" t="n">
+        <v>-6.9531</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>c44</t>
+        </is>
+      </c>
+      <c r="B45" t="n">
+        <v>0.2874</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>c45</t>
+        </is>
+      </c>
+      <c r="B46" t="n">
+        <v>0.3645</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>c46</t>
+        </is>
+      </c>
+      <c r="B47" t="n">
+        <v>1.7383</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>c47</t>
+        </is>
+      </c>
+      <c r="B48" t="n">
+        <v>-1.757</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>c48</t>
+        </is>
+      </c>
+      <c r="B49" t="n">
+        <v>-0.1589</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>c49</t>
+        </is>
+      </c>
+      <c r="B50" t="n">
+        <v>0.3427</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>c50</t>
+        </is>
+      </c>
+      <c r="B51" t="n">
+        <v>-0.2648</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>c51</t>
+        </is>
+      </c>
+      <c r="B52" t="n">
+        <v>0.7164</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>c52</t>
+        </is>
+      </c>
+      <c r="B53" t="n">
+        <v>0.3992</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>c53</t>
+        </is>
+      </c>
+      <c r="B54" t="n">
+        <v>-2.3131</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>c54</t>
+        </is>
+      </c>
+      <c r="B55" t="n">
+        <v>2.853</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>c55</t>
+        </is>
+      </c>
+      <c r="B56" t="n">
+        <v>-3.0991</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>c56</t>
+        </is>
+      </c>
+      <c r="B57" t="n">
+        <v>0.5434</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>c57</t>
+        </is>
+      </c>
+      <c r="B58" t="n">
+        <v>0.9254</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>c58</t>
+        </is>
+      </c>
+      <c r="B59" t="n">
+        <v>-1.2452</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>c59</t>
+        </is>
+      </c>
+      <c r="B60" t="n">
+        <v>1.0553</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>c60</t>
+        </is>
+      </c>
+      <c r="B61" t="n">
+        <v>-0.2932</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>c61</t>
+        </is>
+      </c>
+      <c r="B62" t="n">
+        <v>1.1486</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>c62</t>
+        </is>
+      </c>
+      <c r="B63" t="n">
+        <v>-1.3011</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>c63</t>
+        </is>
+      </c>
+      <c r="B64" t="n">
+        <v>1.0559</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>c64</t>
+        </is>
+      </c>
+      <c r="B65" t="n">
+        <v>-1.0173</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>c65</t>
+        </is>
+      </c>
+      <c r="B66" t="n">
+        <v>0.9917</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>c66</t>
+        </is>
+      </c>
+      <c r="B67" t="n">
+        <v>0.0503</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>c67</t>
+        </is>
+      </c>
+      <c r="B68" t="n">
+        <v>-0.319</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>c68</t>
+        </is>
+      </c>
+      <c r="B69" t="n">
+        <v>0.577</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="inlineStr">
+        <is>
+          <t>c69</t>
+        </is>
+      </c>
+      <c r="B70" t="n">
+        <v>-0.721</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr">
+        <is>
+          <t>c70</t>
+        </is>
+      </c>
+      <c r="B71" t="n">
+        <v>2.7668</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="inlineStr">
+        <is>
+          <t>c71</t>
+        </is>
+      </c>
+      <c r="B72" t="n">
+        <v>-1.3462</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="inlineStr">
+        <is>
+          <t>c72</t>
+        </is>
+      </c>
+      <c r="B73" t="n">
+        <v>-0.3821</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="inlineStr">
+        <is>
+          <t>c73</t>
+        </is>
+      </c>
+      <c r="B74" t="n">
+        <v>-0.1253</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="inlineStr">
+        <is>
+          <t>c74</t>
+        </is>
+      </c>
+      <c r="B75" t="n">
+        <v>0.8832</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="inlineStr">
+        <is>
+          <t>c75</t>
+        </is>
+      </c>
+      <c r="B76" t="n">
+        <v>-0.4076</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="inlineStr">
+        <is>
+          <t>c76</t>
+        </is>
+      </c>
+      <c r="B77" t="n">
+        <v>0.7471</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="inlineStr">
+        <is>
+          <t>c77</t>
+        </is>
+      </c>
+      <c r="B78" t="n">
+        <v>-5.581</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="inlineStr">
+        <is>
+          <t>c78</t>
+        </is>
+      </c>
+      <c r="B79" t="n">
+        <v>21.5768</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="inlineStr">
+        <is>
+          <t>c79</t>
+        </is>
+      </c>
+      <c r="B80" t="n">
+        <v>-11.7261</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="inlineStr">
+        <is>
+          <t>c80</t>
+        </is>
+      </c>
+      <c r="B81" t="n">
+        <v>-19.6725</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="inlineStr">
+        <is>
+          <t>c81</t>
+        </is>
+      </c>
+      <c r="B82" t="n">
+        <v>33.416</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="inlineStr">
+        <is>
+          <t>c82</t>
+        </is>
+      </c>
+      <c r="B83" t="n">
+        <v>-44.9917</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="inlineStr">
+        <is>
+          <t>c83</t>
+        </is>
+      </c>
+      <c r="B84" t="n">
+        <v>29.5506</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="inlineStr">
+        <is>
+          <t>c84</t>
+        </is>
+      </c>
+      <c r="B85" t="n">
+        <v>13.7892</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="inlineStr">
+        <is>
+          <t>c85</t>
+        </is>
+      </c>
+      <c r="B86" t="n">
+        <v>-18.7075</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="inlineStr">
+        <is>
+          <t>c86</t>
+        </is>
+      </c>
+      <c r="B87" t="n">
+        <v>1.0408</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="inlineStr">
+        <is>
+          <t>c87</t>
+        </is>
+      </c>
+      <c r="B88" t="n">
+        <v>5.5445</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="inlineStr">
+        <is>
+          <t>c88</t>
+        </is>
+      </c>
+      <c r="B89" t="n">
+        <v>-14.2186</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="inlineStr">
+        <is>
+          <t>c89</t>
+        </is>
+      </c>
+      <c r="B90" t="n">
+        <v>12.3299</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="inlineStr">
+        <is>
+          <t>c90</t>
+        </is>
+      </c>
+      <c r="B91" t="n">
+        <v>-5.1009</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="inlineStr">
+        <is>
+          <t>c91</t>
+        </is>
+      </c>
+      <c r="B92" t="n">
+        <v>5.0738</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="inlineStr">
+        <is>
+          <t>c92</t>
+        </is>
+      </c>
+      <c r="B93" t="n">
+        <v>-6.1943</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="inlineStr">
+        <is>
+          <t>c93</t>
+        </is>
+      </c>
+      <c r="B94" t="n">
+        <v>7.7033</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="inlineStr">
+        <is>
+          <t>c94</t>
+        </is>
+      </c>
+      <c r="B95" t="n">
+        <v>-9.6191</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="inlineStr">
+        <is>
+          <t>c95</t>
+        </is>
+      </c>
+      <c r="B96" t="n">
+        <v>6.773</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="inlineStr">
+        <is>
+          <t>c96</t>
+        </is>
+      </c>
+      <c r="B97" t="n">
+        <v>-2.473</v>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="inlineStr">
+        <is>
+          <t>c97</t>
+        </is>
+      </c>
+      <c r="B98" t="n">
+        <v>0.119</v>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="inlineStr">
+        <is>
+          <t>c98</t>
+        </is>
+      </c>
+      <c r="B99" t="n">
+        <v>1.9969</v>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="inlineStr">
+        <is>
+          <t>c99</t>
+        </is>
+      </c>
+      <c r="B100" t="n">
+        <v>-2.1065</v>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="inlineStr">
+        <is>
+          <t>c100</t>
+        </is>
+      </c>
+      <c r="B101" t="n">
+        <v>0.4293</v>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" t="inlineStr">
+        <is>
+          <t>c101</t>
+        </is>
+      </c>
+      <c r="B102" t="n">
+        <v>0.3894</v>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="inlineStr">
+        <is>
+          <t>c102</t>
+        </is>
+      </c>
+      <c r="B103" t="n">
+        <v>0.1173</v>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="inlineStr">
+        <is>
+          <t>c103</t>
+        </is>
+      </c>
+      <c r="B104" t="n">
+        <v>-0.1085</v>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" t="inlineStr">
+        <is>
+          <t>c104</t>
+        </is>
+      </c>
+      <c r="B105" t="n">
+        <v>0.3169</v>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" t="inlineStr">
+        <is>
+          <t>c105</t>
+        </is>
+      </c>
+      <c r="B106" t="n">
+        <v>-0.1842</v>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" t="inlineStr">
+        <is>
+          <t>c106</t>
+        </is>
+      </c>
+      <c r="B107" t="n">
+        <v>0.4201</v>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" t="inlineStr">
+        <is>
+          <t>c107</t>
+        </is>
+      </c>
+      <c r="B108" t="n">
+        <v>-1.4961</v>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" t="inlineStr">
+        <is>
+          <t>c108</t>
+        </is>
+      </c>
+      <c r="B109" t="n">
+        <v>11.5645</v>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" t="inlineStr">
+        <is>
+          <t>c109</t>
+        </is>
+      </c>
+      <c r="B110" t="n">
+        <v>-14.7617</v>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" t="inlineStr">
+        <is>
+          <t>c110</t>
+        </is>
+      </c>
+      <c r="B111" t="n">
+        <v>5.4824</v>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" t="inlineStr">
+        <is>
+          <t>c111</t>
+        </is>
+      </c>
+      <c r="B112" t="n">
+        <v>-1.1679</v>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" t="inlineStr">
+        <is>
+          <t>c112</t>
+        </is>
+      </c>
+      <c r="B113" t="n">
+        <v>1.1742</v>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" t="inlineStr">
+        <is>
+          <t>c113</t>
+        </is>
+      </c>
+      <c r="B114" t="n">
+        <v>-2.5707</v>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" t="inlineStr">
+        <is>
+          <t>c114</t>
+        </is>
+      </c>
+      <c r="B115" t="n">
+        <v>0.1086</v>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" t="inlineStr">
+        <is>
+          <t>c115</t>
+        </is>
+      </c>
+      <c r="B116" t="n">
+        <v>0.1752</v>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" t="inlineStr">
+        <is>
+          <t>c116</t>
+        </is>
+      </c>
+      <c r="B117" t="n">
+        <v>-0.1035</v>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" t="inlineStr">
+        <is>
+          <t>c117</t>
+        </is>
+      </c>
+      <c r="B118" t="n">
+        <v>-0.7823</v>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" t="inlineStr">
+        <is>
+          <t>c118</t>
+        </is>
+      </c>
+      <c r="B119" t="n">
+        <v>9.569000000000001</v>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" t="inlineStr">
+        <is>
+          <t>c119</t>
+        </is>
+      </c>
+      <c r="B120" t="n">
+        <v>-16.4937</v>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" t="inlineStr">
+        <is>
+          <t>c120</t>
+        </is>
+      </c>
+      <c r="B121" t="n">
+        <v>8.405799999999999</v>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" t="inlineStr">
+        <is>
+          <t>c121</t>
+        </is>
+      </c>
+      <c r="B122" t="n">
+        <v>-4.9705</v>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123" t="inlineStr">
+        <is>
+          <t>c122</t>
+        </is>
+      </c>
+      <c r="B123" t="n">
+        <v>4.0116</v>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124" t="inlineStr">
+        <is>
+          <t>c123</t>
+        </is>
+      </c>
+      <c r="B124" t="n">
+        <v>-2.076</v>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125" t="inlineStr">
+        <is>
+          <t>c124</t>
+        </is>
+      </c>
+      <c r="B125" t="n">
+        <v>1.2924</v>
+      </c>
+    </row>
+    <row r="126">
+      <c r="A126" t="inlineStr">
+        <is>
+          <t>c125</t>
+        </is>
+      </c>
+      <c r="B126" t="n">
+        <v>-0.09370000000000001</v>
+      </c>
+    </row>
+    <row r="127">
+      <c r="A127" t="inlineStr">
+        <is>
+          <t>c126</t>
+        </is>
+      </c>
+      <c r="B127" t="n">
+        <v>-0.08890000000000001</v>
+      </c>
+    </row>
+    <row r="128">
+      <c r="A128" t="inlineStr">
+        <is>
+          <t>c127</t>
+        </is>
+      </c>
+      <c r="B128" t="n">
+        <v>1.2639</v>
+      </c>
+    </row>
+    <row r="129">
+      <c r="A129" t="inlineStr">
+        <is>
+          <t>c128</t>
+        </is>
+      </c>
+      <c r="B129" t="n">
+        <v>-1.9667</v>
+      </c>
+    </row>
+    <row r="130">
+      <c r="A130" t="inlineStr">
+        <is>
+          <t>c129</t>
+        </is>
+      </c>
+      <c r="B130" t="n">
+        <v>3.6029</v>
+      </c>
+    </row>
+    <row r="131">
+      <c r="A131" t="inlineStr">
+        <is>
+          <t>c130</t>
+        </is>
+      </c>
+      <c r="B131" t="n">
+        <v>-3.4448</v>
+      </c>
+    </row>
+    <row r="132">
+      <c r="A132" t="inlineStr">
+        <is>
+          <t>c131</t>
+        </is>
+      </c>
+      <c r="B132" t="n">
+        <v>1.1762</v>
+      </c>
+    </row>
+    <row r="133">
+      <c r="A133" t="inlineStr">
+        <is>
+          <t>c132</t>
+        </is>
+      </c>
+      <c r="B133" t="n">
+        <v>-1.2599</v>
+      </c>
+    </row>
+    <row r="134">
+      <c r="A134" t="inlineStr">
+        <is>
+          <t>c133</t>
+        </is>
+      </c>
+      <c r="B134" t="n">
+        <v>0.8633999999999999</v>
+      </c>
+    </row>
+    <row r="135">
+      <c r="A135" t="inlineStr">
+        <is>
+          <t>c134</t>
+        </is>
+      </c>
+      <c r="B135" t="n">
+        <v>0.8062</v>
+      </c>
+    </row>
+    <row r="136">
+      <c r="A136" t="inlineStr">
+        <is>
+          <t>c135</t>
+        </is>
+      </c>
+      <c r="B136" t="n">
+        <v>-1.0881</v>
+      </c>
+    </row>
+    <row r="137">
+      <c r="A137" t="inlineStr">
+        <is>
+          <t>c136</t>
+        </is>
+      </c>
+      <c r="B137" t="n">
+        <v>0.5461</v>
+      </c>
+    </row>
+    <row r="138">
+      <c r="A138" t="inlineStr">
+        <is>
+          <t>c137</t>
+        </is>
+      </c>
+      <c r="B138" t="n">
+        <v>-1.0963</v>
+      </c>
+    </row>
+    <row r="139">
+      <c r="A139" t="inlineStr">
+        <is>
+          <t>c138</t>
+        </is>
+      </c>
+      <c r="B139" t="n">
+        <v>0.8391</v>
+      </c>
+    </row>
+    <row r="140">
+      <c r="A140" t="inlineStr">
+        <is>
+          <t>c139</t>
+        </is>
+      </c>
+      <c r="B140" t="n">
+        <v>-0.4693</v>
+      </c>
+    </row>
+    <row r="141">
+      <c r="A141" t="inlineStr">
+        <is>
+          <t>c140</t>
+        </is>
+      </c>
+      <c r="B141" t="n">
+        <v>1.1373</v>
+      </c>
+    </row>
+    <row r="142">
+      <c r="A142" t="inlineStr">
+        <is>
+          <t>c141</t>
+        </is>
+      </c>
+      <c r="B142" t="n">
+        <v>-1.0799</v>
+      </c>
+    </row>
+    <row r="143">
+      <c r="A143" t="inlineStr">
+        <is>
+          <t>c142</t>
+        </is>
+      </c>
+      <c r="B143" t="n">
+        <v>0.1822</v>
+      </c>
+    </row>
+    <row r="144">
+      <c r="A144" t="inlineStr">
+        <is>
+          <t>c143</t>
+        </is>
+      </c>
+      <c r="B144" t="n">
+        <v>0.2548</v>
+      </c>
+    </row>
+    <row r="145">
+      <c r="A145" t="inlineStr">
+        <is>
+          <t>c144</t>
+        </is>
+      </c>
+      <c r="B145" t="n">
+        <v>-1.0849</v>
+      </c>
+    </row>
+    <row r="146">
+      <c r="A146" t="inlineStr">
+        <is>
+          <t>c145</t>
+        </is>
+      </c>
+      <c r="B146" t="n">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>